<commit_message>
First commit from mumbai
</commit_message>
<xml_diff>
--- a/TalentProfileProject/Data/ShareSkill_Data.xlsx
+++ b/TalentProfileProject/Data/ShareSkill_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Renu\Indusconnect\TalentShareSkillProject\TalentProfileProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C878A2-7C8F-4914-AF22-3D719D6C83FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E529BC08-6849-4A1C-ACEE-5022D79852B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,10 +211,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +501,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,10 +582,10 @@
       <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0</v>
       </c>
       <c r="H2" s="1">
@@ -597,7 +600,7 @@
       <c r="K2" t="s">
         <v>30</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -623,10 +626,10 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" s="1">
@@ -641,7 +644,7 @@
       <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>2</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -667,10 +670,10 @@
       <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4" s="1">
@@ -685,7 +688,7 @@
       <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>3</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -711,10 +714,10 @@
       <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>1</v>
       </c>
       <c r="H5" s="1">
@@ -729,7 +732,7 @@
       <c r="K5" t="s">
         <v>33</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <v>4</v>
       </c>
       <c r="M5" s="2" t="s">

</xml_diff>